<commit_message>
Removed duns information from the spec files
</commit_message>
<xml_diff>
--- a/_apidocs/entity-api/v1/v2_CSV_Response.xlsx
+++ b/_apidocs/entity-api/v1/v2_CSV_Response.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MATTFINNELL\git\open-gsa-redesign\_apidocs\entity-api\v1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BhargavBoppana\IdeaProjects\open-gsa-redesign1\_apidocs\entity-api\v1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E5350079-A530-4BAF-BC83-BEEA794DFF85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D5FC98-FDA3-44AF-B6E6-B18A7A99E0EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560"/>
+    <workbookView xWindow="4092" yWindow="2340" windowWidth="16584" windowHeight="9468" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Example6-Entity (3)" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="373">
   <si>
     <t>samRegistered</t>
   </si>
@@ -28,9 +28,6 @@
     <t>ueiSAM</t>
   </si>
   <si>
-    <t>ueiDUNS</t>
-  </si>
-  <si>
     <t>entityEFTIndicator</t>
   </si>
   <si>
@@ -89,9 +86,6 @@
   </si>
   <si>
     <t>immediateParentEntity.ueiSAM</t>
-  </si>
-  <si>
-    <t>immediateParentEntity.ueiDUNS</t>
   </si>
   <si>
     <t>immediateParentEntity.legalBusinessName</t>
@@ -1150,7 +1144,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1986,14 +1980,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:MG2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:ME2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="W1" sqref="W1:W1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:345" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:343" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3023,280 +3019,274 @@
       <c r="ME1" t="s">
         <v>342</v>
       </c>
-      <c r="MF1" t="s">
+    </row>
+    <row r="2" spans="1:343" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>343</v>
       </c>
-      <c r="MG1" t="s">
+      <c r="B2" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="2" spans="1:345" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>345</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>345</v>
+      </c>
+      <c r="D2" t="s">
         <v>346</v>
       </c>
-      <c r="C2">
-        <v>709741482</v>
-      </c>
-      <c r="D2" t="s">
-        <v>347</v>
-      </c>
       <c r="E2" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="F2" t="s">
         <v>347</v>
       </c>
       <c r="G2" t="s">
+        <v>345</v>
+      </c>
+      <c r="H2" t="s">
+        <v>348</v>
+      </c>
+      <c r="I2" t="s">
         <v>349</v>
       </c>
-      <c r="H2" t="s">
-        <v>347</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>350</v>
       </c>
-      <c r="J2" t="s">
-        <v>351</v>
-      </c>
-      <c r="K2" t="s">
-        <v>352</v>
+      <c r="K2" s="1">
+        <v>44379</v>
       </c>
       <c r="L2" s="1">
         <v>44379</v>
       </c>
       <c r="M2" s="1">
+        <v>44744</v>
+      </c>
+      <c r="N2" s="1">
         <v>44379</v>
       </c>
-      <c r="N2" s="1">
+      <c r="O2" t="s">
+        <v>350</v>
+      </c>
+      <c r="P2" s="1">
         <v>44744</v>
       </c>
-      <c r="O2" s="1">
+      <c r="Q2" s="1">
         <v>44379</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
+        <v>351</v>
+      </c>
+      <c r="S2" t="s">
+        <v>345</v>
+      </c>
+      <c r="T2" t="s">
+        <v>345</v>
+      </c>
+      <c r="U2" t="s">
+        <v>351</v>
+      </c>
+      <c r="V2" t="s">
+        <v>345</v>
+      </c>
+      <c r="W2" t="s">
+        <v>345</v>
+      </c>
+      <c r="X2" t="s">
+        <v>345</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>345</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>345</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>345</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>345</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>345</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>345</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>345</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>345</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>345</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>345</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>345</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>345</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>345</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>345</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>345</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>345</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>345</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>345</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>345</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>345</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>345</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>345</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>345</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>345</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>345</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>345</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>345</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>345</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>345</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>345</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>345</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>345</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>345</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>345</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>345</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>345</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>345</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>345</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>345</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>345</v>
+      </c>
+      <c r="BM2" t="s">
         <v>352</v>
       </c>
-      <c r="Q2" s="1">
-        <v>44744</v>
-      </c>
-      <c r="R2" s="1">
+      <c r="BN2" t="s">
+        <v>352</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>352</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>352</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>352</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>352</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>352</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>352</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>352</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>352</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>352</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>345</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>345</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>345</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>345</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>345</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>345</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>345</v>
+      </c>
+      <c r="CE2" t="s">
+        <v>345</v>
+      </c>
+      <c r="CF2" t="s">
+        <v>345</v>
+      </c>
+      <c r="CG2" s="1">
+        <v>29160</v>
+      </c>
+      <c r="CH2" s="2">
+        <v>44500</v>
+      </c>
+      <c r="CI2" s="1">
         <v>44379</v>
       </c>
-      <c r="S2" t="s">
+      <c r="CJ2" t="s">
         <v>353</v>
       </c>
-      <c r="T2" t="s">
-        <v>347</v>
-      </c>
-      <c r="U2" t="s">
-        <v>347</v>
-      </c>
-      <c r="V2" t="s">
-        <v>353</v>
-      </c>
-      <c r="W2" t="s">
-        <v>347</v>
-      </c>
-      <c r="X2" t="s">
-        <v>347</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>347</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>347</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>347</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>347</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>347</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>347</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>347</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>347</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>347</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>347</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>347</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>347</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>347</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>347</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>347</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>347</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>347</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>347</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>347</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>347</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>347</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>347</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>347</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>347</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>347</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>347</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>347</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>347</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>347</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>347</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>347</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>347</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>347</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>347</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>347</v>
-      </c>
-      <c r="BH2" t="s">
-        <v>347</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>347</v>
-      </c>
-      <c r="BJ2" t="s">
-        <v>347</v>
-      </c>
-      <c r="BK2" t="s">
-        <v>347</v>
-      </c>
-      <c r="BL2" t="s">
-        <v>347</v>
-      </c>
-      <c r="BM2" t="s">
-        <v>347</v>
-      </c>
-      <c r="BN2" t="s">
-        <v>347</v>
-      </c>
-      <c r="BO2" t="s">
+      <c r="CK2" t="s">
         <v>354</v>
-      </c>
-      <c r="BP2" t="s">
-        <v>354</v>
-      </c>
-      <c r="BQ2" t="s">
-        <v>354</v>
-      </c>
-      <c r="BR2" t="s">
-        <v>354</v>
-      </c>
-      <c r="BS2" t="s">
-        <v>354</v>
-      </c>
-      <c r="BT2" t="s">
-        <v>354</v>
-      </c>
-      <c r="BU2" t="s">
-        <v>354</v>
-      </c>
-      <c r="BV2" t="s">
-        <v>354</v>
-      </c>
-      <c r="BW2" t="s">
-        <v>354</v>
-      </c>
-      <c r="BX2" t="s">
-        <v>354</v>
-      </c>
-      <c r="BY2" t="s">
-        <v>354</v>
-      </c>
-      <c r="BZ2" t="s">
-        <v>347</v>
-      </c>
-      <c r="CA2" t="s">
-        <v>347</v>
-      </c>
-      <c r="CB2" t="s">
-        <v>347</v>
-      </c>
-      <c r="CC2" t="s">
-        <v>347</v>
-      </c>
-      <c r="CD2" t="s">
-        <v>347</v>
-      </c>
-      <c r="CE2" t="s">
-        <v>347</v>
-      </c>
-      <c r="CF2" t="s">
-        <v>347</v>
-      </c>
-      <c r="CG2" t="s">
-        <v>347</v>
-      </c>
-      <c r="CH2" t="s">
-        <v>347</v>
-      </c>
-      <c r="CI2" s="1">
-        <v>29160</v>
-      </c>
-      <c r="CJ2" s="2">
-        <v>44500</v>
-      </c>
-      <c r="CK2" s="1">
-        <v>44379</v>
       </c>
       <c r="CL2" t="s">
         <v>355</v>
@@ -3304,20 +3294,20 @@
       <c r="CM2" t="s">
         <v>356</v>
       </c>
-      <c r="CN2" t="s">
+      <c r="CN2">
+        <v>11111</v>
+      </c>
+      <c r="CO2">
+        <v>1111</v>
+      </c>
+      <c r="CP2" t="s">
         <v>357</v>
       </c>
-      <c r="CO2" t="s">
-        <v>358</v>
-      </c>
-      <c r="CP2">
-        <v>11111</v>
-      </c>
-      <c r="CQ2">
-        <v>1111</v>
+      <c r="CQ2" t="s">
+        <v>353</v>
       </c>
       <c r="CR2" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="CS2" t="s">
         <v>355</v>
@@ -3325,29 +3315,29 @@
       <c r="CT2" t="s">
         <v>356</v>
       </c>
-      <c r="CU2" t="s">
+      <c r="CU2">
+        <v>11111</v>
+      </c>
+      <c r="CV2">
+        <v>1111</v>
+      </c>
+      <c r="CW2" t="s">
         <v>357</v>
       </c>
-      <c r="CV2" t="s">
+      <c r="CX2">
+        <v>0</v>
+      </c>
+      <c r="CY2" t="s">
+        <v>345</v>
+      </c>
+      <c r="CZ2" t="s">
+        <v>345</v>
+      </c>
+      <c r="DA2" t="s">
         <v>358</v>
       </c>
-      <c r="CW2">
-        <v>11111</v>
-      </c>
-      <c r="CX2">
-        <v>1111</v>
-      </c>
-      <c r="CY2" t="s">
+      <c r="DB2" t="s">
         <v>359</v>
-      </c>
-      <c r="CZ2">
-        <v>0</v>
-      </c>
-      <c r="DA2" t="s">
-        <v>347</v>
-      </c>
-      <c r="DB2" t="s">
-        <v>347</v>
       </c>
       <c r="DC2" t="s">
         <v>360</v>
@@ -3362,175 +3352,175 @@
         <v>363</v>
       </c>
       <c r="DG2" t="s">
+        <v>345</v>
+      </c>
+      <c r="DH2" t="s">
+        <v>345</v>
+      </c>
+      <c r="DI2" t="s">
+        <v>345</v>
+      </c>
+      <c r="DJ2" t="s">
+        <v>345</v>
+      </c>
+      <c r="DK2" t="s">
         <v>364</v>
       </c>
-      <c r="DH2" t="s">
+      <c r="DL2" t="s">
         <v>365</v>
       </c>
-      <c r="DI2" t="s">
-        <v>347</v>
-      </c>
-      <c r="DJ2" t="s">
-        <v>347</v>
-      </c>
-      <c r="DK2" t="s">
-        <v>347</v>
-      </c>
-      <c r="DL2" t="s">
-        <v>347</v>
-      </c>
       <c r="DM2" t="s">
+        <v>345</v>
+      </c>
+      <c r="DN2" t="s">
+        <v>345</v>
+      </c>
+      <c r="DO2" t="s">
+        <v>345</v>
+      </c>
+      <c r="DP2" t="s">
+        <v>345</v>
+      </c>
+      <c r="DQ2" t="s">
         <v>366</v>
       </c>
-      <c r="DN2" t="s">
+      <c r="DR2" t="s">
         <v>367</v>
       </c>
-      <c r="DO2" t="s">
-        <v>347</v>
-      </c>
-      <c r="DP2" t="s">
-        <v>347</v>
-      </c>
-      <c r="DQ2" t="s">
-        <v>347</v>
-      </c>
-      <c r="DR2" t="s">
-        <v>347</v>
-      </c>
       <c r="DS2" t="s">
+        <v>345</v>
+      </c>
+      <c r="DT2" t="s">
+        <v>345</v>
+      </c>
+      <c r="DU2" t="s">
+        <v>345</v>
+      </c>
+      <c r="DV2" t="s">
+        <v>345</v>
+      </c>
+      <c r="DW2" t="s">
         <v>368</v>
       </c>
-      <c r="DT2" t="s">
+      <c r="DX2" t="s">
+        <v>345</v>
+      </c>
+      <c r="DY2" t="s">
+        <v>345</v>
+      </c>
+      <c r="DZ2" t="s">
+        <v>345</v>
+      </c>
+      <c r="EA2" t="s">
+        <v>345</v>
+      </c>
+      <c r="EB2" t="s">
+        <v>345</v>
+      </c>
+      <c r="EC2" t="s">
+        <v>345</v>
+      </c>
+      <c r="ED2" t="s">
+        <v>345</v>
+      </c>
+      <c r="EE2" t="s">
+        <v>345</v>
+      </c>
+      <c r="EF2" t="s">
+        <v>345</v>
+      </c>
+      <c r="EG2" t="s">
+        <v>345</v>
+      </c>
+      <c r="EH2" t="s">
+        <v>345</v>
+      </c>
+      <c r="EI2" t="s">
+        <v>345</v>
+      </c>
+      <c r="EJ2" t="s">
+        <v>345</v>
+      </c>
+      <c r="EK2" t="s">
+        <v>345</v>
+      </c>
+      <c r="EL2" t="s">
+        <v>345</v>
+      </c>
+      <c r="EM2" t="s">
+        <v>345</v>
+      </c>
+      <c r="EN2" t="s">
+        <v>345</v>
+      </c>
+      <c r="EO2" t="s">
+        <v>345</v>
+      </c>
+      <c r="EP2" t="s">
+        <v>345</v>
+      </c>
+      <c r="EQ2" t="s">
+        <v>345</v>
+      </c>
+      <c r="ER2" t="s">
+        <v>345</v>
+      </c>
+      <c r="ES2" t="s">
+        <v>345</v>
+      </c>
+      <c r="ET2" t="s">
+        <v>345</v>
+      </c>
+      <c r="EU2" t="s">
+        <v>345</v>
+      </c>
+      <c r="EV2" t="s">
+        <v>345</v>
+      </c>
+      <c r="EW2" t="s">
+        <v>345</v>
+      </c>
+      <c r="EX2" t="s">
+        <v>345</v>
+      </c>
+      <c r="EY2" t="s">
+        <v>345</v>
+      </c>
+      <c r="EZ2" t="s">
+        <v>345</v>
+      </c>
+      <c r="FA2" t="s">
         <v>369</v>
       </c>
-      <c r="DU2" t="s">
-        <v>347</v>
-      </c>
-      <c r="DV2" t="s">
-        <v>347</v>
-      </c>
-      <c r="DW2" t="s">
-        <v>347</v>
-      </c>
-      <c r="DX2" t="s">
-        <v>347</v>
-      </c>
-      <c r="DY2" t="s">
+      <c r="FB2" t="s">
+        <v>345</v>
+      </c>
+      <c r="FC2" t="s">
         <v>370</v>
       </c>
-      <c r="DZ2" t="s">
-        <v>347</v>
-      </c>
-      <c r="EA2" t="s">
-        <v>347</v>
-      </c>
-      <c r="EB2" t="s">
-        <v>347</v>
-      </c>
-      <c r="EC2" t="s">
-        <v>347</v>
-      </c>
-      <c r="ED2" t="s">
-        <v>347</v>
-      </c>
-      <c r="EE2" t="s">
-        <v>347</v>
-      </c>
-      <c r="EF2" t="s">
-        <v>347</v>
-      </c>
-      <c r="EG2" t="s">
-        <v>347</v>
-      </c>
-      <c r="EH2" t="s">
-        <v>347</v>
-      </c>
-      <c r="EI2" t="s">
-        <v>347</v>
-      </c>
-      <c r="EJ2" t="s">
-        <v>347</v>
-      </c>
-      <c r="EK2" t="s">
-        <v>347</v>
-      </c>
-      <c r="EL2" t="s">
-        <v>347</v>
-      </c>
-      <c r="EM2" t="s">
-        <v>347</v>
-      </c>
-      <c r="EN2" t="s">
-        <v>347</v>
-      </c>
-      <c r="EO2" t="s">
-        <v>347</v>
-      </c>
-      <c r="EP2" t="s">
-        <v>347</v>
-      </c>
-      <c r="EQ2" t="s">
-        <v>347</v>
-      </c>
-      <c r="ER2" t="s">
-        <v>347</v>
-      </c>
-      <c r="ES2" t="s">
-        <v>347</v>
-      </c>
-      <c r="ET2" t="s">
-        <v>347</v>
-      </c>
-      <c r="EU2" t="s">
-        <v>347</v>
-      </c>
-      <c r="EV2" t="s">
-        <v>347</v>
-      </c>
-      <c r="EW2" t="s">
-        <v>347</v>
-      </c>
-      <c r="EX2" t="s">
-        <v>347</v>
-      </c>
-      <c r="EY2" t="s">
-        <v>347</v>
-      </c>
-      <c r="EZ2" t="s">
-        <v>347</v>
-      </c>
-      <c r="FA2" t="s">
-        <v>347</v>
-      </c>
-      <c r="FB2" t="s">
-        <v>347</v>
-      </c>
-      <c r="FC2" t="s">
+      <c r="FD2" t="s">
         <v>371</v>
       </c>
-      <c r="FD2" t="s">
-        <v>347</v>
-      </c>
-      <c r="FE2" t="s">
-        <v>372</v>
-      </c>
-      <c r="FF2" t="s">
-        <v>373</v>
+      <c r="FE2">
+        <v>1234567890</v>
+      </c>
+      <c r="FF2">
+        <v>1234</v>
       </c>
       <c r="FG2">
         <v>1234567890</v>
       </c>
-      <c r="FH2">
-        <v>1234</v>
-      </c>
-      <c r="FI2">
-        <v>1234567890</v>
+      <c r="FH2" t="s">
+        <v>345</v>
+      </c>
+      <c r="FI2" t="s">
+        <v>372</v>
       </c>
       <c r="FJ2" t="s">
-        <v>347</v>
+        <v>353</v>
       </c>
       <c r="FK2" t="s">
-        <v>374</v>
+        <v>354</v>
       </c>
       <c r="FL2" t="s">
         <v>355</v>
@@ -3538,47 +3528,47 @@
       <c r="FM2" t="s">
         <v>356</v>
       </c>
-      <c r="FN2" t="s">
+      <c r="FN2">
+        <v>11111</v>
+      </c>
+      <c r="FO2">
+        <v>1111</v>
+      </c>
+      <c r="FP2" t="s">
         <v>357</v>
       </c>
-      <c r="FO2" t="s">
-        <v>358</v>
-      </c>
-      <c r="FP2">
-        <v>11111</v>
-      </c>
-      <c r="FQ2">
-        <v>1111</v>
+      <c r="FQ2" t="s">
+        <v>369</v>
       </c>
       <c r="FR2" t="s">
-        <v>359</v>
+        <v>345</v>
       </c>
       <c r="FS2" t="s">
+        <v>370</v>
+      </c>
+      <c r="FT2" t="s">
         <v>371</v>
       </c>
-      <c r="FT2" t="s">
-        <v>347</v>
-      </c>
-      <c r="FU2" t="s">
-        <v>372</v>
-      </c>
-      <c r="FV2" t="s">
-        <v>373</v>
+      <c r="FU2">
+        <v>1234567890</v>
+      </c>
+      <c r="FV2">
+        <v>1234</v>
       </c>
       <c r="FW2">
         <v>1234567890</v>
       </c>
-      <c r="FX2">
-        <v>1234</v>
-      </c>
-      <c r="FY2">
-        <v>1234567890</v>
+      <c r="FX2" t="s">
+        <v>345</v>
+      </c>
+      <c r="FY2" t="s">
+        <v>372</v>
       </c>
       <c r="FZ2" t="s">
-        <v>347</v>
+        <v>353</v>
       </c>
       <c r="GA2" t="s">
-        <v>374</v>
+        <v>354</v>
       </c>
       <c r="GB2" t="s">
         <v>355</v>
@@ -3586,485 +3576,479 @@
       <c r="GC2" t="s">
         <v>356</v>
       </c>
-      <c r="GD2" t="s">
+      <c r="GD2">
+        <v>11111</v>
+      </c>
+      <c r="GE2">
+        <v>1111</v>
+      </c>
+      <c r="GF2" t="s">
         <v>357</v>
       </c>
-      <c r="GE2" t="s">
-        <v>358</v>
-      </c>
-      <c r="GF2">
-        <v>11111</v>
-      </c>
-      <c r="GG2">
-        <v>1111</v>
+      <c r="GG2" t="s">
+        <v>345</v>
       </c>
       <c r="GH2" t="s">
-        <v>359</v>
+        <v>345</v>
       </c>
       <c r="GI2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="GJ2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="GK2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="GL2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="GM2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="GN2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="GO2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="GP2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="GQ2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="GR2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="GS2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="GT2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="GU2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="GV2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="GW2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="GX2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="GY2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="GZ2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="HA2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="HB2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="HC2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="HD2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="HE2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="HF2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="HG2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="HH2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="HI2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="HJ2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="HK2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="HL2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="HM2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="HN2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="HO2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="HP2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="HQ2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="HR2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="HS2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="HT2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="HU2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="HV2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="HW2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="HX2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="HY2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="HZ2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="IA2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="IB2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="IC2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="ID2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="IE2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="IF2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="IG2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="IH2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="II2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="IJ2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="IK2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="IL2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="IM2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="IN2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="IO2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="IP2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="IQ2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="IR2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="IS2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="IT2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="IU2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="IV2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="IW2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="IX2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="IY2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="IZ2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="JA2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="JB2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="JC2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="JD2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="JE2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="JF2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="JG2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="JH2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="JI2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="JJ2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="JK2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="JL2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="JM2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="JN2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="JO2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="JP2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="JQ2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="JR2" t="s">
-        <v>347</v>
+        <v>369</v>
       </c>
       <c r="JS2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="JT2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="JU2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="JV2" t="s">
+        <v>345</v>
+      </c>
+      <c r="JW2" t="s">
+        <v>345</v>
+      </c>
+      <c r="JX2">
+        <v>1234567890</v>
+      </c>
+      <c r="JY2" t="s">
+        <v>345</v>
+      </c>
+      <c r="JZ2" t="s">
         <v>372</v>
       </c>
-      <c r="JW2" t="s">
-        <v>347</v>
-      </c>
-      <c r="JX2" t="s">
-        <v>347</v>
-      </c>
-      <c r="JY2" t="s">
-        <v>347</v>
-      </c>
-      <c r="JZ2">
-        <v>1234567890</v>
-      </c>
       <c r="KA2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="KB2" t="s">
-        <v>374</v>
+        <v>345</v>
       </c>
       <c r="KC2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="KD2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="KE2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="KF2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="KG2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="KH2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="KI2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="KJ2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="KK2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="KL2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="KM2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="KN2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="KO2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="KP2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="KQ2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="KR2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="KS2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="KT2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="KU2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="KV2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="KW2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="KX2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="KY2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="KZ2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="LA2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="LB2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="LC2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="LD2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="LE2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="LF2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="LG2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="LH2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="LI2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="LJ2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="LK2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="LL2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="LM2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="LN2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="LO2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="LP2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="LQ2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="LR2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="LS2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="LT2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="LU2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="LV2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="LW2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="LX2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="LY2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="LZ2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="MA2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="MB2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="MC2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="MD2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="ME2" t="s">
-        <v>347</v>
-      </c>
-      <c r="MF2" t="s">
-        <v>347</v>
-      </c>
-      <c r="MG2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated changes for removal duns
</commit_message>
<xml_diff>
--- a/_apidocs/entity-api/v1/v2_CSV_Response.xlsx
+++ b/_apidocs/entity-api/v1/v2_CSV_Response.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BhargavBoppana\IdeaProjects\open-gsa-redesign1\_apidocs\entity-api\v1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D5FC98-FDA3-44AF-B6E6-B18A7A99E0EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1B0B75-9D4A-4114-9E56-133FB5C0C061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4092" yWindow="2340" windowWidth="16584" windowHeight="9468" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="372">
   <si>
     <t>samRegistered</t>
   </si>
@@ -116,9 +116,6 @@
   </si>
   <si>
     <t>domesticParent.ueiSAM</t>
-  </si>
-  <si>
-    <t>domesticParent.ueiDUNS</t>
   </si>
   <si>
     <t>domesticParent.legalBusinessName</t>
@@ -1981,15 +1978,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:ME2"/>
+  <dimension ref="A1:MD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="W1" sqref="W1:W1048576"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AG1" sqref="AG1:AG1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:343" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:342" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3016,40 +3013,37 @@
       <c r="MD1" t="s">
         <v>341</v>
       </c>
-      <c r="ME1" t="s">
+    </row>
+    <row r="2" spans="1:342" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="2" spans="1:343" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>343</v>
       </c>
-      <c r="B2" t="s">
-        <v>344</v>
-      </c>
       <c r="C2" t="s">
+        <v>344</v>
+      </c>
+      <c r="D2" t="s">
         <v>345</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>344</v>
+      </c>
+      <c r="F2" t="s">
         <v>346</v>
       </c>
-      <c r="E2" t="s">
-        <v>345</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>344</v>
+      </c>
+      <c r="H2" t="s">
         <v>347</v>
       </c>
-      <c r="G2" t="s">
-        <v>345</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>348</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>349</v>
-      </c>
-      <c r="J2" t="s">
-        <v>350</v>
       </c>
       <c r="K2" s="1">
         <v>44379</v>
@@ -3064,7 +3058,7 @@
         <v>44379</v>
       </c>
       <c r="O2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="P2" s="1">
         <v>44744</v>
@@ -3073,214 +3067,214 @@
         <v>44379</v>
       </c>
       <c r="R2" t="s">
+        <v>350</v>
+      </c>
+      <c r="S2" t="s">
+        <v>344</v>
+      </c>
+      <c r="T2" t="s">
+        <v>344</v>
+      </c>
+      <c r="U2" t="s">
+        <v>350</v>
+      </c>
+      <c r="V2" t="s">
+        <v>344</v>
+      </c>
+      <c r="W2" t="s">
+        <v>344</v>
+      </c>
+      <c r="X2" t="s">
+        <v>344</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>344</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>344</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>344</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>344</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>344</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>344</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>344</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>344</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>344</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>344</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>344</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>344</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>344</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>344</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>344</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>344</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>344</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>344</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>344</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>344</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>344</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>344</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>344</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>344</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>344</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>344</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>344</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>344</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>344</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>344</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>344</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>344</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>344</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>344</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>344</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>344</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>344</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>344</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>344</v>
+      </c>
+      <c r="BL2" t="s">
         <v>351</v>
       </c>
-      <c r="S2" t="s">
-        <v>345</v>
-      </c>
-      <c r="T2" t="s">
-        <v>345</v>
-      </c>
-      <c r="U2" t="s">
+      <c r="BM2" t="s">
         <v>351</v>
       </c>
-      <c r="V2" t="s">
-        <v>345</v>
-      </c>
-      <c r="W2" t="s">
-        <v>345</v>
-      </c>
-      <c r="X2" t="s">
-        <v>345</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>345</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>345</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>345</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>345</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>345</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>345</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>345</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>345</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>345</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>345</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>345</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>345</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>345</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>345</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>345</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>345</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>345</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>345</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>345</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>345</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>345</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>345</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>345</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>345</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>345</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>345</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>345</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>345</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>345</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>345</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>345</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>345</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>345</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>345</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>345</v>
-      </c>
-      <c r="BH2" t="s">
-        <v>345</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>345</v>
-      </c>
-      <c r="BJ2" t="s">
-        <v>345</v>
-      </c>
-      <c r="BK2" t="s">
-        <v>345</v>
-      </c>
-      <c r="BL2" t="s">
-        <v>345</v>
-      </c>
-      <c r="BM2" t="s">
+      <c r="BN2" t="s">
+        <v>351</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>351</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>351</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>351</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>351</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>351</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>351</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>351</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>351</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>344</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>344</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>344</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>344</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>344</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>344</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>344</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>344</v>
+      </c>
+      <c r="CE2" t="s">
+        <v>344</v>
+      </c>
+      <c r="CF2" s="1">
+        <v>29160</v>
+      </c>
+      <c r="CG2" s="2">
+        <v>44500</v>
+      </c>
+      <c r="CH2" s="1">
+        <v>44379</v>
+      </c>
+      <c r="CI2" t="s">
         <v>352</v>
-      </c>
-      <c r="BN2" t="s">
-        <v>352</v>
-      </c>
-      <c r="BO2" t="s">
-        <v>352</v>
-      </c>
-      <c r="BP2" t="s">
-        <v>352</v>
-      </c>
-      <c r="BQ2" t="s">
-        <v>352</v>
-      </c>
-      <c r="BR2" t="s">
-        <v>352</v>
-      </c>
-      <c r="BS2" t="s">
-        <v>352</v>
-      </c>
-      <c r="BT2" t="s">
-        <v>352</v>
-      </c>
-      <c r="BU2" t="s">
-        <v>352</v>
-      </c>
-      <c r="BV2" t="s">
-        <v>352</v>
-      </c>
-      <c r="BW2" t="s">
-        <v>352</v>
-      </c>
-      <c r="BX2" t="s">
-        <v>345</v>
-      </c>
-      <c r="BY2" t="s">
-        <v>345</v>
-      </c>
-      <c r="BZ2" t="s">
-        <v>345</v>
-      </c>
-      <c r="CA2" t="s">
-        <v>345</v>
-      </c>
-      <c r="CB2" t="s">
-        <v>345</v>
-      </c>
-      <c r="CC2" t="s">
-        <v>345</v>
-      </c>
-      <c r="CD2" t="s">
-        <v>345</v>
-      </c>
-      <c r="CE2" t="s">
-        <v>345</v>
-      </c>
-      <c r="CF2" t="s">
-        <v>345</v>
-      </c>
-      <c r="CG2" s="1">
-        <v>29160</v>
-      </c>
-      <c r="CH2" s="2">
-        <v>44500</v>
-      </c>
-      <c r="CI2" s="1">
-        <v>44379</v>
       </c>
       <c r="CJ2" t="s">
         <v>353</v>
@@ -3291,17 +3285,17 @@
       <c r="CL2" t="s">
         <v>355</v>
       </c>
-      <c r="CM2" t="s">
+      <c r="CM2">
+        <v>11111</v>
+      </c>
+      <c r="CN2">
+        <v>1111</v>
+      </c>
+      <c r="CO2" t="s">
         <v>356</v>
       </c>
-      <c r="CN2">
-        <v>11111</v>
-      </c>
-      <c r="CO2">
-        <v>1111</v>
-      </c>
       <c r="CP2" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="CQ2" t="s">
         <v>353</v>
@@ -3312,26 +3306,26 @@
       <c r="CS2" t="s">
         <v>355</v>
       </c>
-      <c r="CT2" t="s">
+      <c r="CT2">
+        <v>11111</v>
+      </c>
+      <c r="CU2">
+        <v>1111</v>
+      </c>
+      <c r="CV2" t="s">
         <v>356</v>
       </c>
-      <c r="CU2">
-        <v>11111</v>
-      </c>
-      <c r="CV2">
-        <v>1111</v>
-      </c>
-      <c r="CW2" t="s">
+      <c r="CW2">
+        <v>0</v>
+      </c>
+      <c r="CX2" t="s">
+        <v>344</v>
+      </c>
+      <c r="CY2" t="s">
+        <v>344</v>
+      </c>
+      <c r="CZ2" t="s">
         <v>357</v>
-      </c>
-      <c r="CX2">
-        <v>0</v>
-      </c>
-      <c r="CY2" t="s">
-        <v>345</v>
-      </c>
-      <c r="CZ2" t="s">
-        <v>345</v>
       </c>
       <c r="DA2" t="s">
         <v>358</v>
@@ -3349,172 +3343,172 @@
         <v>362</v>
       </c>
       <c r="DF2" t="s">
+        <v>344</v>
+      </c>
+      <c r="DG2" t="s">
+        <v>344</v>
+      </c>
+      <c r="DH2" t="s">
+        <v>344</v>
+      </c>
+      <c r="DI2" t="s">
+        <v>344</v>
+      </c>
+      <c r="DJ2" t="s">
         <v>363</v>
-      </c>
-      <c r="DG2" t="s">
-        <v>345</v>
-      </c>
-      <c r="DH2" t="s">
-        <v>345</v>
-      </c>
-      <c r="DI2" t="s">
-        <v>345</v>
-      </c>
-      <c r="DJ2" t="s">
-        <v>345</v>
       </c>
       <c r="DK2" t="s">
         <v>364</v>
       </c>
       <c r="DL2" t="s">
+        <v>344</v>
+      </c>
+      <c r="DM2" t="s">
+        <v>344</v>
+      </c>
+      <c r="DN2" t="s">
+        <v>344</v>
+      </c>
+      <c r="DO2" t="s">
+        <v>344</v>
+      </c>
+      <c r="DP2" t="s">
         <v>365</v>
-      </c>
-      <c r="DM2" t="s">
-        <v>345</v>
-      </c>
-      <c r="DN2" t="s">
-        <v>345</v>
-      </c>
-      <c r="DO2" t="s">
-        <v>345</v>
-      </c>
-      <c r="DP2" t="s">
-        <v>345</v>
       </c>
       <c r="DQ2" t="s">
         <v>366</v>
       </c>
       <c r="DR2" t="s">
+        <v>344</v>
+      </c>
+      <c r="DS2" t="s">
+        <v>344</v>
+      </c>
+      <c r="DT2" t="s">
+        <v>344</v>
+      </c>
+      <c r="DU2" t="s">
+        <v>344</v>
+      </c>
+      <c r="DV2" t="s">
         <v>367</v>
       </c>
-      <c r="DS2" t="s">
-        <v>345</v>
-      </c>
-      <c r="DT2" t="s">
-        <v>345</v>
-      </c>
-      <c r="DU2" t="s">
-        <v>345</v>
-      </c>
-      <c r="DV2" t="s">
-        <v>345</v>
-      </c>
       <c r="DW2" t="s">
+        <v>344</v>
+      </c>
+      <c r="DX2" t="s">
+        <v>344</v>
+      </c>
+      <c r="DY2" t="s">
+        <v>344</v>
+      </c>
+      <c r="DZ2" t="s">
+        <v>344</v>
+      </c>
+      <c r="EA2" t="s">
+        <v>344</v>
+      </c>
+      <c r="EB2" t="s">
+        <v>344</v>
+      </c>
+      <c r="EC2" t="s">
+        <v>344</v>
+      </c>
+      <c r="ED2" t="s">
+        <v>344</v>
+      </c>
+      <c r="EE2" t="s">
+        <v>344</v>
+      </c>
+      <c r="EF2" t="s">
+        <v>344</v>
+      </c>
+      <c r="EG2" t="s">
+        <v>344</v>
+      </c>
+      <c r="EH2" t="s">
+        <v>344</v>
+      </c>
+      <c r="EI2" t="s">
+        <v>344</v>
+      </c>
+      <c r="EJ2" t="s">
+        <v>344</v>
+      </c>
+      <c r="EK2" t="s">
+        <v>344</v>
+      </c>
+      <c r="EL2" t="s">
+        <v>344</v>
+      </c>
+      <c r="EM2" t="s">
+        <v>344</v>
+      </c>
+      <c r="EN2" t="s">
+        <v>344</v>
+      </c>
+      <c r="EO2" t="s">
+        <v>344</v>
+      </c>
+      <c r="EP2" t="s">
+        <v>344</v>
+      </c>
+      <c r="EQ2" t="s">
+        <v>344</v>
+      </c>
+      <c r="ER2" t="s">
+        <v>344</v>
+      </c>
+      <c r="ES2" t="s">
+        <v>344</v>
+      </c>
+      <c r="ET2" t="s">
+        <v>344</v>
+      </c>
+      <c r="EU2" t="s">
+        <v>344</v>
+      </c>
+      <c r="EV2" t="s">
+        <v>344</v>
+      </c>
+      <c r="EW2" t="s">
+        <v>344</v>
+      </c>
+      <c r="EX2" t="s">
+        <v>344</v>
+      </c>
+      <c r="EY2" t="s">
+        <v>344</v>
+      </c>
+      <c r="EZ2" t="s">
         <v>368</v>
       </c>
-      <c r="DX2" t="s">
-        <v>345</v>
-      </c>
-      <c r="DY2" t="s">
-        <v>345</v>
-      </c>
-      <c r="DZ2" t="s">
-        <v>345</v>
-      </c>
-      <c r="EA2" t="s">
-        <v>345</v>
-      </c>
-      <c r="EB2" t="s">
-        <v>345</v>
-      </c>
-      <c r="EC2" t="s">
-        <v>345</v>
-      </c>
-      <c r="ED2" t="s">
-        <v>345</v>
-      </c>
-      <c r="EE2" t="s">
-        <v>345</v>
-      </c>
-      <c r="EF2" t="s">
-        <v>345</v>
-      </c>
-      <c r="EG2" t="s">
-        <v>345</v>
-      </c>
-      <c r="EH2" t="s">
-        <v>345</v>
-      </c>
-      <c r="EI2" t="s">
-        <v>345</v>
-      </c>
-      <c r="EJ2" t="s">
-        <v>345</v>
-      </c>
-      <c r="EK2" t="s">
-        <v>345</v>
-      </c>
-      <c r="EL2" t="s">
-        <v>345</v>
-      </c>
-      <c r="EM2" t="s">
-        <v>345</v>
-      </c>
-      <c r="EN2" t="s">
-        <v>345</v>
-      </c>
-      <c r="EO2" t="s">
-        <v>345</v>
-      </c>
-      <c r="EP2" t="s">
-        <v>345</v>
-      </c>
-      <c r="EQ2" t="s">
-        <v>345</v>
-      </c>
-      <c r="ER2" t="s">
-        <v>345</v>
-      </c>
-      <c r="ES2" t="s">
-        <v>345</v>
-      </c>
-      <c r="ET2" t="s">
-        <v>345</v>
-      </c>
-      <c r="EU2" t="s">
-        <v>345</v>
-      </c>
-      <c r="EV2" t="s">
-        <v>345</v>
-      </c>
-      <c r="EW2" t="s">
-        <v>345</v>
-      </c>
-      <c r="EX2" t="s">
-        <v>345</v>
-      </c>
-      <c r="EY2" t="s">
-        <v>345</v>
-      </c>
-      <c r="EZ2" t="s">
-        <v>345</v>
-      </c>
       <c r="FA2" t="s">
+        <v>344</v>
+      </c>
+      <c r="FB2" t="s">
         <v>369</v>
-      </c>
-      <c r="FB2" t="s">
-        <v>345</v>
       </c>
       <c r="FC2" t="s">
         <v>370</v>
       </c>
-      <c r="FD2" t="s">
+      <c r="FD2">
+        <v>1234567890</v>
+      </c>
+      <c r="FE2">
+        <v>1234</v>
+      </c>
+      <c r="FF2">
+        <v>1234567890</v>
+      </c>
+      <c r="FG2" t="s">
+        <v>344</v>
+      </c>
+      <c r="FH2" t="s">
         <v>371</v>
       </c>
-      <c r="FE2">
-        <v>1234567890</v>
-      </c>
-      <c r="FF2">
-        <v>1234</v>
-      </c>
-      <c r="FG2">
-        <v>1234567890</v>
-      </c>
-      <c r="FH2" t="s">
-        <v>345</v>
-      </c>
       <c r="FI2" t="s">
-        <v>372</v>
+        <v>352</v>
       </c>
       <c r="FJ2" t="s">
         <v>353</v>
@@ -3525,44 +3519,44 @@
       <c r="FL2" t="s">
         <v>355</v>
       </c>
-      <c r="FM2" t="s">
+      <c r="FM2">
+        <v>11111</v>
+      </c>
+      <c r="FN2">
+        <v>1111</v>
+      </c>
+      <c r="FO2" t="s">
         <v>356</v>
       </c>
-      <c r="FN2">
-        <v>11111</v>
-      </c>
-      <c r="FO2">
-        <v>1111</v>
-      </c>
       <c r="FP2" t="s">
-        <v>357</v>
+        <v>368</v>
       </c>
       <c r="FQ2" t="s">
+        <v>344</v>
+      </c>
+      <c r="FR2" t="s">
         <v>369</v>
-      </c>
-      <c r="FR2" t="s">
-        <v>345</v>
       </c>
       <c r="FS2" t="s">
         <v>370</v>
       </c>
-      <c r="FT2" t="s">
+      <c r="FT2">
+        <v>1234567890</v>
+      </c>
+      <c r="FU2">
+        <v>1234</v>
+      </c>
+      <c r="FV2">
+        <v>1234567890</v>
+      </c>
+      <c r="FW2" t="s">
+        <v>344</v>
+      </c>
+      <c r="FX2" t="s">
         <v>371</v>
       </c>
-      <c r="FU2">
-        <v>1234567890</v>
-      </c>
-      <c r="FV2">
-        <v>1234</v>
-      </c>
-      <c r="FW2">
-        <v>1234567890</v>
-      </c>
-      <c r="FX2" t="s">
-        <v>345</v>
-      </c>
       <c r="FY2" t="s">
-        <v>372</v>
+        <v>352</v>
       </c>
       <c r="FZ2" t="s">
         <v>353</v>
@@ -3573,482 +3567,479 @@
       <c r="GB2" t="s">
         <v>355</v>
       </c>
-      <c r="GC2" t="s">
+      <c r="GC2">
+        <v>11111</v>
+      </c>
+      <c r="GD2">
+        <v>1111</v>
+      </c>
+      <c r="GE2" t="s">
         <v>356</v>
       </c>
-      <c r="GD2">
-        <v>11111</v>
-      </c>
-      <c r="GE2">
-        <v>1111</v>
-      </c>
       <c r="GF2" t="s">
-        <v>357</v>
+        <v>344</v>
       </c>
       <c r="GG2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="GH2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="GI2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="GJ2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="GK2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="GL2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="GM2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="GN2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="GO2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="GP2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="GQ2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="GR2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="GS2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="GT2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="GU2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="GV2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="GW2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="GX2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="GY2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="GZ2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="HA2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="HB2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="HC2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="HD2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="HE2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="HF2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="HG2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="HH2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="HI2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="HJ2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="HK2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="HL2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="HM2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="HN2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="HO2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="HP2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="HQ2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="HR2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="HS2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="HT2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="HU2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="HV2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="HW2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="HX2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="HY2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="HZ2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="IA2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="IB2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="IC2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="ID2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="IE2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="IF2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="IG2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="IH2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="II2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="IJ2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="IK2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="IL2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="IM2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="IN2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="IO2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="IP2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="IQ2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="IR2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="IS2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="IT2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="IU2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="IV2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="IW2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="IX2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="IY2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="IZ2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="JA2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="JB2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="JC2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="JD2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="JE2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="JF2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="JG2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="JH2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="JI2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="JJ2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="JK2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="JL2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="JM2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="JN2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="JO2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="JP2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="JQ2" t="s">
-        <v>345</v>
+        <v>368</v>
       </c>
       <c r="JR2" t="s">
+        <v>344</v>
+      </c>
+      <c r="JS2" t="s">
         <v>369</v>
       </c>
-      <c r="JS2" t="s">
-        <v>345</v>
-      </c>
       <c r="JT2" t="s">
-        <v>370</v>
+        <v>344</v>
       </c>
       <c r="JU2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="JV2" t="s">
-        <v>345</v>
-      </c>
-      <c r="JW2" t="s">
-        <v>345</v>
-      </c>
-      <c r="JX2">
+        <v>344</v>
+      </c>
+      <c r="JW2">
         <v>1234567890</v>
       </c>
+      <c r="JX2" t="s">
+        <v>344</v>
+      </c>
       <c r="JY2" t="s">
-        <v>345</v>
+        <v>371</v>
       </c>
       <c r="JZ2" t="s">
-        <v>372</v>
+        <v>344</v>
       </c>
       <c r="KA2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="KB2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="KC2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="KD2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="KE2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="KF2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="KG2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="KH2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="KI2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="KJ2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="KK2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="KL2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="KM2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="KN2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="KO2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="KP2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="KQ2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="KR2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="KS2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="KT2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="KU2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="KV2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="KW2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="KX2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="KY2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="KZ2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="LA2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="LB2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="LC2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="LD2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="LE2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="LF2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="LG2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="LH2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="LI2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="LJ2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="LK2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="LL2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="LM2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="LN2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="LO2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="LP2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="LQ2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="LR2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="LS2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="LT2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="LU2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="LV2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="LW2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="LX2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="LY2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="LZ2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="MA2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="MB2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="MC2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="MD2" t="s">
-        <v>345</v>
-      </c>
-      <c r="ME2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added proper extract layout files
</commit_message>
<xml_diff>
--- a/_apidocs/entity-api/v1/v2_CSV_Response.xlsx
+++ b/_apidocs/entity-api/v1/v2_CSV_Response.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BhargavBoppana\IdeaProjects\open-gsa-redesign1\_apidocs\entity-api\v1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1B0B75-9D4A-4114-9E56-133FB5C0C061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302E030D-8A02-412D-8545-7C72D99DA3C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4092" yWindow="2340" windowWidth="16584" windowHeight="9468" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="370">
   <si>
     <t>samRegistered</t>
   </si>
@@ -148,9 +148,6 @@
     <t>hqParent.ueiSAM</t>
   </si>
   <si>
-    <t>hqParent.ueiDUNS</t>
-  </si>
-  <si>
     <t>hqParent.legalBusinessName</t>
   </si>
   <si>
@@ -179,9 +176,6 @@
   </si>
   <si>
     <t>ultimateParentEntity.ueiSAM</t>
-  </si>
-  <si>
-    <t>ultimateParentEntity.ueiDUNS</t>
   </si>
   <si>
     <t>ultimateParentEntity.legalBusinessName</t>
@@ -1978,15 +1972,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:MD2"/>
+  <dimension ref="A1:MB2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AG1" sqref="AG1:AG1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:342" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3007,43 +2999,37 @@
       <c r="MB1" t="s">
         <v>339</v>
       </c>
-      <c r="MC1" t="s">
+    </row>
+    <row r="2" spans="1:340" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>340</v>
       </c>
-      <c r="MD1" t="s">
+      <c r="B2" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="2" spans="1:342" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>342</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>342</v>
+      </c>
+      <c r="D2" t="s">
         <v>343</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
+        <v>342</v>
+      </c>
+      <c r="F2" t="s">
         <v>344</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
+        <v>342</v>
+      </c>
+      <c r="H2" t="s">
         <v>345</v>
       </c>
-      <c r="E2" t="s">
-        <v>344</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>346</v>
       </c>
-      <c r="G2" t="s">
-        <v>344</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>347</v>
-      </c>
-      <c r="I2" t="s">
-        <v>348</v>
-      </c>
-      <c r="J2" t="s">
-        <v>349</v>
       </c>
       <c r="K2" s="1">
         <v>44379</v>
@@ -3058,7 +3044,7 @@
         <v>44379</v>
       </c>
       <c r="O2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="P2" s="1">
         <v>44744</v>
@@ -3067,211 +3053,211 @@
         <v>44379</v>
       </c>
       <c r="R2" t="s">
+        <v>348</v>
+      </c>
+      <c r="S2" t="s">
+        <v>342</v>
+      </c>
+      <c r="T2" t="s">
+        <v>342</v>
+      </c>
+      <c r="U2" t="s">
+        <v>348</v>
+      </c>
+      <c r="V2" t="s">
+        <v>342</v>
+      </c>
+      <c r="W2" t="s">
+        <v>342</v>
+      </c>
+      <c r="X2" t="s">
+        <v>342</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>342</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>342</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>342</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>342</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>342</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>342</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>342</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>342</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>342</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>342</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>342</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>342</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>342</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>342</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>342</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>342</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>342</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>342</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>342</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>342</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>342</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>342</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>342</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>342</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>342</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>342</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>342</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>342</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>342</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>342</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>342</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>342</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>342</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>342</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>342</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>342</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>349</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>349</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>349</v>
+      </c>
+      <c r="BM2" t="s">
+        <v>349</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>349</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>349</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>349</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>349</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>349</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>349</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>349</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>342</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>342</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>342</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>342</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>342</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>342</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>342</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>342</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>342</v>
+      </c>
+      <c r="CD2" s="1">
+        <v>29160</v>
+      </c>
+      <c r="CE2" s="2">
+        <v>44500</v>
+      </c>
+      <c r="CF2" s="1">
+        <v>44379</v>
+      </c>
+      <c r="CG2" t="s">
         <v>350</v>
       </c>
-      <c r="S2" t="s">
-        <v>344</v>
-      </c>
-      <c r="T2" t="s">
-        <v>344</v>
-      </c>
-      <c r="U2" t="s">
-        <v>350</v>
-      </c>
-      <c r="V2" t="s">
-        <v>344</v>
-      </c>
-      <c r="W2" t="s">
-        <v>344</v>
-      </c>
-      <c r="X2" t="s">
-        <v>344</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>344</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>344</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>344</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>344</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>344</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>344</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>344</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>344</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>344</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>344</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>344</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>344</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>344</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>344</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>344</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>344</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>344</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>344</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>344</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>344</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>344</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>344</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>344</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>344</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>344</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>344</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>344</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>344</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>344</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>344</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>344</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>344</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>344</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>344</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>344</v>
-      </c>
-      <c r="BH2" t="s">
-        <v>344</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>344</v>
-      </c>
-      <c r="BJ2" t="s">
-        <v>344</v>
-      </c>
-      <c r="BK2" t="s">
-        <v>344</v>
-      </c>
-      <c r="BL2" t="s">
+      <c r="CH2" t="s">
         <v>351</v>
-      </c>
-      <c r="BM2" t="s">
-        <v>351</v>
-      </c>
-      <c r="BN2" t="s">
-        <v>351</v>
-      </c>
-      <c r="BO2" t="s">
-        <v>351</v>
-      </c>
-      <c r="BP2" t="s">
-        <v>351</v>
-      </c>
-      <c r="BQ2" t="s">
-        <v>351</v>
-      </c>
-      <c r="BR2" t="s">
-        <v>351</v>
-      </c>
-      <c r="BS2" t="s">
-        <v>351</v>
-      </c>
-      <c r="BT2" t="s">
-        <v>351</v>
-      </c>
-      <c r="BU2" t="s">
-        <v>351</v>
-      </c>
-      <c r="BV2" t="s">
-        <v>351</v>
-      </c>
-      <c r="BW2" t="s">
-        <v>344</v>
-      </c>
-      <c r="BX2" t="s">
-        <v>344</v>
-      </c>
-      <c r="BY2" t="s">
-        <v>344</v>
-      </c>
-      <c r="BZ2" t="s">
-        <v>344</v>
-      </c>
-      <c r="CA2" t="s">
-        <v>344</v>
-      </c>
-      <c r="CB2" t="s">
-        <v>344</v>
-      </c>
-      <c r="CC2" t="s">
-        <v>344</v>
-      </c>
-      <c r="CD2" t="s">
-        <v>344</v>
-      </c>
-      <c r="CE2" t="s">
-        <v>344</v>
-      </c>
-      <c r="CF2" s="1">
-        <v>29160</v>
-      </c>
-      <c r="CG2" s="2">
-        <v>44500</v>
-      </c>
-      <c r="CH2" s="1">
-        <v>44379</v>
       </c>
       <c r="CI2" t="s">
         <v>352</v>
@@ -3279,20 +3265,20 @@
       <c r="CJ2" t="s">
         <v>353</v>
       </c>
-      <c r="CK2" t="s">
+      <c r="CK2">
+        <v>11111</v>
+      </c>
+      <c r="CL2">
+        <v>1111</v>
+      </c>
+      <c r="CM2" t="s">
         <v>354</v>
       </c>
-      <c r="CL2" t="s">
-        <v>355</v>
-      </c>
-      <c r="CM2">
-        <v>11111</v>
-      </c>
-      <c r="CN2">
-        <v>1111</v>
+      <c r="CN2" t="s">
+        <v>350</v>
       </c>
       <c r="CO2" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="CP2" t="s">
         <v>352</v>
@@ -3300,29 +3286,29 @@
       <c r="CQ2" t="s">
         <v>353</v>
       </c>
-      <c r="CR2" t="s">
+      <c r="CR2">
+        <v>11111</v>
+      </c>
+      <c r="CS2">
+        <v>1111</v>
+      </c>
+      <c r="CT2" t="s">
         <v>354</v>
       </c>
-      <c r="CS2" t="s">
+      <c r="CU2">
+        <v>0</v>
+      </c>
+      <c r="CV2" t="s">
+        <v>342</v>
+      </c>
+      <c r="CW2" t="s">
+        <v>342</v>
+      </c>
+      <c r="CX2" t="s">
         <v>355</v>
       </c>
-      <c r="CT2">
-        <v>11111</v>
-      </c>
-      <c r="CU2">
-        <v>1111</v>
-      </c>
-      <c r="CV2" t="s">
+      <c r="CY2" t="s">
         <v>356</v>
-      </c>
-      <c r="CW2">
-        <v>0</v>
-      </c>
-      <c r="CX2" t="s">
-        <v>344</v>
-      </c>
-      <c r="CY2" t="s">
-        <v>344</v>
       </c>
       <c r="CZ2" t="s">
         <v>357</v>
@@ -3337,175 +3323,175 @@
         <v>360</v>
       </c>
       <c r="DD2" t="s">
+        <v>342</v>
+      </c>
+      <c r="DE2" t="s">
+        <v>342</v>
+      </c>
+      <c r="DF2" t="s">
+        <v>342</v>
+      </c>
+      <c r="DG2" t="s">
+        <v>342</v>
+      </c>
+      <c r="DH2" t="s">
         <v>361</v>
       </c>
-      <c r="DE2" t="s">
+      <c r="DI2" t="s">
         <v>362</v>
       </c>
-      <c r="DF2" t="s">
-        <v>344</v>
-      </c>
-      <c r="DG2" t="s">
-        <v>344</v>
-      </c>
-      <c r="DH2" t="s">
-        <v>344</v>
-      </c>
-      <c r="DI2" t="s">
-        <v>344</v>
-      </c>
       <c r="DJ2" t="s">
+        <v>342</v>
+      </c>
+      <c r="DK2" t="s">
+        <v>342</v>
+      </c>
+      <c r="DL2" t="s">
+        <v>342</v>
+      </c>
+      <c r="DM2" t="s">
+        <v>342</v>
+      </c>
+      <c r="DN2" t="s">
         <v>363</v>
       </c>
-      <c r="DK2" t="s">
+      <c r="DO2" t="s">
         <v>364</v>
       </c>
-      <c r="DL2" t="s">
-        <v>344</v>
-      </c>
-      <c r="DM2" t="s">
-        <v>344</v>
-      </c>
-      <c r="DN2" t="s">
-        <v>344</v>
-      </c>
-      <c r="DO2" t="s">
-        <v>344</v>
-      </c>
       <c r="DP2" t="s">
+        <v>342</v>
+      </c>
+      <c r="DQ2" t="s">
+        <v>342</v>
+      </c>
+      <c r="DR2" t="s">
+        <v>342</v>
+      </c>
+      <c r="DS2" t="s">
+        <v>342</v>
+      </c>
+      <c r="DT2" t="s">
         <v>365</v>
       </c>
-      <c r="DQ2" t="s">
+      <c r="DU2" t="s">
+        <v>342</v>
+      </c>
+      <c r="DV2" t="s">
+        <v>342</v>
+      </c>
+      <c r="DW2" t="s">
+        <v>342</v>
+      </c>
+      <c r="DX2" t="s">
+        <v>342</v>
+      </c>
+      <c r="DY2" t="s">
+        <v>342</v>
+      </c>
+      <c r="DZ2" t="s">
+        <v>342</v>
+      </c>
+      <c r="EA2" t="s">
+        <v>342</v>
+      </c>
+      <c r="EB2" t="s">
+        <v>342</v>
+      </c>
+      <c r="EC2" t="s">
+        <v>342</v>
+      </c>
+      <c r="ED2" t="s">
+        <v>342</v>
+      </c>
+      <c r="EE2" t="s">
+        <v>342</v>
+      </c>
+      <c r="EF2" t="s">
+        <v>342</v>
+      </c>
+      <c r="EG2" t="s">
+        <v>342</v>
+      </c>
+      <c r="EH2" t="s">
+        <v>342</v>
+      </c>
+      <c r="EI2" t="s">
+        <v>342</v>
+      </c>
+      <c r="EJ2" t="s">
+        <v>342</v>
+      </c>
+      <c r="EK2" t="s">
+        <v>342</v>
+      </c>
+      <c r="EL2" t="s">
+        <v>342</v>
+      </c>
+      <c r="EM2" t="s">
+        <v>342</v>
+      </c>
+      <c r="EN2" t="s">
+        <v>342</v>
+      </c>
+      <c r="EO2" t="s">
+        <v>342</v>
+      </c>
+      <c r="EP2" t="s">
+        <v>342</v>
+      </c>
+      <c r="EQ2" t="s">
+        <v>342</v>
+      </c>
+      <c r="ER2" t="s">
+        <v>342</v>
+      </c>
+      <c r="ES2" t="s">
+        <v>342</v>
+      </c>
+      <c r="ET2" t="s">
+        <v>342</v>
+      </c>
+      <c r="EU2" t="s">
+        <v>342</v>
+      </c>
+      <c r="EV2" t="s">
+        <v>342</v>
+      </c>
+      <c r="EW2" t="s">
+        <v>342</v>
+      </c>
+      <c r="EX2" t="s">
         <v>366</v>
       </c>
-      <c r="DR2" t="s">
-        <v>344</v>
-      </c>
-      <c r="DS2" t="s">
-        <v>344</v>
-      </c>
-      <c r="DT2" t="s">
-        <v>344</v>
-      </c>
-      <c r="DU2" t="s">
-        <v>344</v>
-      </c>
-      <c r="DV2" t="s">
+      <c r="EY2" t="s">
+        <v>342</v>
+      </c>
+      <c r="EZ2" t="s">
         <v>367</v>
       </c>
-      <c r="DW2" t="s">
-        <v>344</v>
-      </c>
-      <c r="DX2" t="s">
-        <v>344</v>
-      </c>
-      <c r="DY2" t="s">
-        <v>344</v>
-      </c>
-      <c r="DZ2" t="s">
-        <v>344</v>
-      </c>
-      <c r="EA2" t="s">
-        <v>344</v>
-      </c>
-      <c r="EB2" t="s">
-        <v>344</v>
-      </c>
-      <c r="EC2" t="s">
-        <v>344</v>
-      </c>
-      <c r="ED2" t="s">
-        <v>344</v>
-      </c>
-      <c r="EE2" t="s">
-        <v>344</v>
-      </c>
-      <c r="EF2" t="s">
-        <v>344</v>
-      </c>
-      <c r="EG2" t="s">
-        <v>344</v>
-      </c>
-      <c r="EH2" t="s">
-        <v>344</v>
-      </c>
-      <c r="EI2" t="s">
-        <v>344</v>
-      </c>
-      <c r="EJ2" t="s">
-        <v>344</v>
-      </c>
-      <c r="EK2" t="s">
-        <v>344</v>
-      </c>
-      <c r="EL2" t="s">
-        <v>344</v>
-      </c>
-      <c r="EM2" t="s">
-        <v>344</v>
-      </c>
-      <c r="EN2" t="s">
-        <v>344</v>
-      </c>
-      <c r="EO2" t="s">
-        <v>344</v>
-      </c>
-      <c r="EP2" t="s">
-        <v>344</v>
-      </c>
-      <c r="EQ2" t="s">
-        <v>344</v>
-      </c>
-      <c r="ER2" t="s">
-        <v>344</v>
-      </c>
-      <c r="ES2" t="s">
-        <v>344</v>
-      </c>
-      <c r="ET2" t="s">
-        <v>344</v>
-      </c>
-      <c r="EU2" t="s">
-        <v>344</v>
-      </c>
-      <c r="EV2" t="s">
-        <v>344</v>
-      </c>
-      <c r="EW2" t="s">
-        <v>344</v>
-      </c>
-      <c r="EX2" t="s">
-        <v>344</v>
-      </c>
-      <c r="EY2" t="s">
-        <v>344</v>
-      </c>
-      <c r="EZ2" t="s">
+      <c r="FA2" t="s">
         <v>368</v>
       </c>
-      <c r="FA2" t="s">
-        <v>344</v>
-      </c>
-      <c r="FB2" t="s">
-        <v>369</v>
-      </c>
-      <c r="FC2" t="s">
-        <v>370</v>
+      <c r="FB2">
+        <v>1234567890</v>
+      </c>
+      <c r="FC2">
+        <v>1234</v>
       </c>
       <c r="FD2">
         <v>1234567890</v>
       </c>
-      <c r="FE2">
-        <v>1234</v>
-      </c>
-      <c r="FF2">
-        <v>1234567890</v>
+      <c r="FE2" t="s">
+        <v>342</v>
+      </c>
+      <c r="FF2" t="s">
+        <v>369</v>
       </c>
       <c r="FG2" t="s">
-        <v>344</v>
+        <v>350</v>
       </c>
       <c r="FH2" t="s">
-        <v>371</v>
+        <v>351</v>
       </c>
       <c r="FI2" t="s">
         <v>352</v>
@@ -3513,47 +3499,47 @@
       <c r="FJ2" t="s">
         <v>353</v>
       </c>
-      <c r="FK2" t="s">
+      <c r="FK2">
+        <v>11111</v>
+      </c>
+      <c r="FL2">
+        <v>1111</v>
+      </c>
+      <c r="FM2" t="s">
         <v>354</v>
       </c>
-      <c r="FL2" t="s">
-        <v>355</v>
-      </c>
-      <c r="FM2">
-        <v>11111</v>
-      </c>
-      <c r="FN2">
-        <v>1111</v>
+      <c r="FN2" t="s">
+        <v>366</v>
       </c>
       <c r="FO2" t="s">
-        <v>356</v>
+        <v>342</v>
       </c>
       <c r="FP2" t="s">
+        <v>367</v>
+      </c>
+      <c r="FQ2" t="s">
         <v>368</v>
       </c>
-      <c r="FQ2" t="s">
-        <v>344</v>
-      </c>
-      <c r="FR2" t="s">
-        <v>369</v>
-      </c>
-      <c r="FS2" t="s">
-        <v>370</v>
+      <c r="FR2">
+        <v>1234567890</v>
+      </c>
+      <c r="FS2">
+        <v>1234</v>
       </c>
       <c r="FT2">
         <v>1234567890</v>
       </c>
-      <c r="FU2">
-        <v>1234</v>
-      </c>
-      <c r="FV2">
-        <v>1234567890</v>
+      <c r="FU2" t="s">
+        <v>342</v>
+      </c>
+      <c r="FV2" t="s">
+        <v>369</v>
       </c>
       <c r="FW2" t="s">
-        <v>344</v>
+        <v>350</v>
       </c>
       <c r="FX2" t="s">
-        <v>371</v>
+        <v>351</v>
       </c>
       <c r="FY2" t="s">
         <v>352</v>
@@ -3561,485 +3547,479 @@
       <c r="FZ2" t="s">
         <v>353</v>
       </c>
-      <c r="GA2" t="s">
+      <c r="GA2">
+        <v>11111</v>
+      </c>
+      <c r="GB2">
+        <v>1111</v>
+      </c>
+      <c r="GC2" t="s">
         <v>354</v>
       </c>
-      <c r="GB2" t="s">
-        <v>355</v>
-      </c>
-      <c r="GC2">
-        <v>11111</v>
-      </c>
-      <c r="GD2">
-        <v>1111</v>
+      <c r="GD2" t="s">
+        <v>342</v>
       </c>
       <c r="GE2" t="s">
-        <v>356</v>
+        <v>342</v>
       </c>
       <c r="GF2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="GG2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="GH2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="GI2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="GJ2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="GK2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="GL2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="GM2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="GN2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="GO2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="GP2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="GQ2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="GR2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="GS2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="GT2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="GU2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="GV2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="GW2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="GX2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="GY2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="GZ2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="HA2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="HB2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="HC2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="HD2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="HE2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="HF2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="HG2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="HH2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="HI2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="HJ2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="HK2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="HL2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="HM2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="HN2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="HO2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="HP2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="HQ2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="HR2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="HS2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="HT2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="HU2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="HV2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="HW2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="HX2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="HY2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="HZ2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="IA2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="IB2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="IC2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="ID2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="IE2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="IF2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="IG2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="IH2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="II2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="IJ2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="IK2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="IL2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="IM2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="IN2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="IO2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="IP2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="IQ2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="IR2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="IS2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="IT2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="IU2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="IV2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="IW2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="IX2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="IY2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="IZ2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="JA2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="JB2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="JC2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="JD2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="JE2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="JF2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="JG2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="JH2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="JI2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="JJ2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="JK2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="JL2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="JM2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="JN2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="JO2" t="s">
-        <v>344</v>
+        <v>366</v>
       </c>
       <c r="JP2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="JQ2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="JR2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="JS2" t="s">
+        <v>342</v>
+      </c>
+      <c r="JT2" t="s">
+        <v>342</v>
+      </c>
+      <c r="JU2">
+        <v>1234567890</v>
+      </c>
+      <c r="JV2" t="s">
+        <v>342</v>
+      </c>
+      <c r="JW2" t="s">
         <v>369</v>
       </c>
-      <c r="JT2" t="s">
-        <v>344</v>
-      </c>
-      <c r="JU2" t="s">
-        <v>344</v>
-      </c>
-      <c r="JV2" t="s">
-        <v>344</v>
-      </c>
-      <c r="JW2">
-        <v>1234567890</v>
-      </c>
       <c r="JX2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="JY2" t="s">
-        <v>371</v>
+        <v>342</v>
       </c>
       <c r="JZ2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="KA2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="KB2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="KC2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="KD2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="KE2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="KF2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="KG2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="KH2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="KI2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="KJ2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="KK2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="KL2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="KM2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="KN2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="KO2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="KP2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="KQ2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="KR2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="KS2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="KT2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="KU2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="KV2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="KW2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="KX2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="KY2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="KZ2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="LA2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="LB2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="LC2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="LD2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="LE2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="LF2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="LG2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="LH2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="LI2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="LJ2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="LK2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="LL2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="LM2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="LN2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="LO2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="LP2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="LQ2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="LR2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="LS2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="LT2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="LU2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="LV2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="LW2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="LX2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="LY2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="LZ2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="MA2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="MB2" t="s">
-        <v>344</v>
-      </c>
-      <c r="MC2" t="s">
-        <v>344</v>
-      </c>
-      <c r="MD2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
   </sheetData>

</xml_diff>